<commit_message>
Added to continuity circuit
</commit_message>
<xml_diff>
--- a/Documentation/Features.xlsx
+++ b/Documentation/Features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angus McLennan\Documents\1. Uni Work\HPR\Strelka-Flight-Computer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angus McLennan\Documents\1. Uni Work\HPR\Strelka-Flight-Computer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F1719C-412D-4A70-9A52-0C6EA3C3F9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C699071-69D9-4F1F-90CA-81F025A8E3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Feature</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Brownout protection</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Status LEDs</t>
   </si>
 </sst>
 </file>
@@ -585,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D6:F14"/>
+  <dimension ref="D6:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,6 +661,16 @@
     <row r="14" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>